<commit_message>
cambios en el frotn
</commit_message>
<xml_diff>
--- a/apps/api/data/PROGRAMA_DE_MANTENIMIENTO_PREVENTIVO.xlsx
+++ b/apps/api/data/PROGRAMA_DE_MANTENIMIENTO_PREVENTIVO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andregb/Documents/WORK/IMA DOCS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andregb/Documents/WORK/IMA/apps/api/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{271C9DA7-D130-024C-9179-6E2906C33EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC8280E-0564-0A46-925C-6E647023AE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="20740" windowHeight="11040" firstSheet="4" activeTab="5" xr2:uid="{03F6895E-1BE2-41F5-981C-385596757CDF}"/>
+    <workbookView xWindow="-20" yWindow="680" windowWidth="29400" windowHeight="18440" firstSheet="2" activeTab="7" xr2:uid="{03F6895E-1BE2-41F5-981C-385596757CDF}"/>
   </bookViews>
   <sheets>
     <sheet name="MANTENIMIENTO ADICIONAL" sheetId="8" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="MANTENIMIENTO 3 MESES" sheetId="5" r:id="rId5"/>
     <sheet name="MANTENIMIENTO 6 MESES" sheetId="2" r:id="rId6"/>
     <sheet name="MANTENIMIENTO 1 AÑO" sheetId="3" r:id="rId7"/>
-    <sheet name="MANTENIMIENTO MAS DE 1AÑO" sheetId="7" r:id="rId8"/>
+    <sheet name="MANTENIMIENTO MAS DE 1AÑO" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,14 +43,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="208">
   <si>
     <t>EQUIPO DE LA GUIA/TRABAJO DE VIA</t>
   </si>
   <si>
-    <t>Diario</t>
-  </si>
-  <si>
     <t xml:space="preserve">Inspección y mantenimiento etapa l del riel de deslizamiento. </t>
   </si>
   <si>
@@ -112,33 +109,6 @@
   </si>
   <si>
     <t>EQUIPO DE MANTENIMIENTO</t>
-  </si>
-  <si>
-    <t>SEMANAL</t>
-  </si>
-  <si>
-    <t>3MESES</t>
-  </si>
-  <si>
-    <t>1MES</t>
-  </si>
-  <si>
-    <t>4 AÑOS</t>
-  </si>
-  <si>
-    <t>4AÑOS</t>
-  </si>
-  <si>
-    <t>6 AÑOS</t>
-  </si>
-  <si>
-    <t>2 AÑOS</t>
-  </si>
-  <si>
-    <t>5 AÑOS</t>
-  </si>
-  <si>
-    <t>3 AÑOIS</t>
   </si>
   <si>
     <t xml:space="preserve">Inspección visual riel de puerta </t>
@@ -704,6 +674,33 @@
   </si>
   <si>
     <t xml:space="preserve">Inspección y mantenimiento etapa III del servidor </t>
+  </si>
+  <si>
+    <t>1S</t>
+  </si>
+  <si>
+    <t>1D</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>3M</t>
+  </si>
+  <si>
+    <t>4A</t>
+  </si>
+  <si>
+    <t>6A</t>
+  </si>
+  <si>
+    <t>3A</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>5A</t>
   </si>
 </sst>
 </file>
@@ -766,7 +763,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -1079,21 +1076,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color indexed="64"/>
       </left>
@@ -1102,32 +1084,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1160,7 +1116,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1234,9 +1190,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -1248,9 +1201,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1272,13 +1222,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1288,9 +1238,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1393,7 +1340,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1744,7 +1691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5F468F0-E091-4C00-A93E-E0934F835D9D}">
   <dimension ref="B1:E25"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -1752,261 +1699,261 @@
   <cols>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
     <col min="3" max="3" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="123.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="123.6640625" style="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
-        <v>35</v>
+      <c r="B2" s="57" t="s">
+        <v>25</v>
       </c>
       <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="46" t="s">
-        <v>37</v>
+      <c r="D2" s="42" t="s">
+        <v>27</v>
       </c>
       <c r="E2" s="21"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="63"/>
+      <c r="B3" s="58"/>
       <c r="C3" s="2">
         <v>2</v>
       </c>
-      <c r="D3" s="45" t="s">
-        <v>38</v>
+      <c r="D3" s="41" t="s">
+        <v>28</v>
       </c>
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="63"/>
+      <c r="B4" s="58"/>
       <c r="C4" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="45" t="s">
-        <v>36</v>
+      <c r="D4" s="41" t="s">
+        <v>26</v>
       </c>
       <c r="E4" s="17"/>
     </row>
     <row r="5" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="64"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="30">
         <v>4</v>
       </c>
-      <c r="D5" s="47" t="s">
-        <v>39</v>
+      <c r="D5" s="43" t="s">
+        <v>29</v>
       </c>
       <c r="E5" s="20"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="65" t="s">
-        <v>40</v>
+      <c r="B6" s="60" t="s">
+        <v>30</v>
       </c>
       <c r="C6" s="7">
         <v>1</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E6" s="21"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="66"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="2">
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="E7" s="17"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="66"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="2">
         <v>3</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E8" s="17"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="66"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="2">
         <v>4</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E9" s="17"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="66"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="2">
         <v>5</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E10" s="17"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="66"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="2">
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="E11" s="17"/>
     </row>
     <row r="12" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="66"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="30">
         <v>7</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E12" s="20"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="62" t="s">
-        <v>6</v>
+      <c r="B13" s="57" t="s">
+        <v>5</v>
       </c>
       <c r="C13" s="7">
         <v>1</v>
       </c>
-      <c r="D13" s="48" t="s">
-        <v>48</v>
+      <c r="D13" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="E13" s="21"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="63"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="2">
         <v>2</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="E14" s="17"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="63"/>
+      <c r="B15" s="58"/>
       <c r="C15" s="2">
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E15" s="17"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="63"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="2">
         <v>4</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E16" s="17"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="63"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="2">
         <v>5</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E17" s="17"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="63"/>
+      <c r="B18" s="58"/>
       <c r="C18" s="2">
         <v>6</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="E18" s="17"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="63"/>
+      <c r="B19" s="58"/>
       <c r="C19" s="2">
         <v>7</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E19" s="17"/>
     </row>
     <row r="20" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="64"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="30">
         <v>8</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="E20" s="20"/>
     </row>
     <row r="21" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="49">
+        <v>46</v>
+      </c>
+      <c r="C21" s="45">
         <v>1</v>
       </c>
-      <c r="D21" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="51"/>
+      <c r="D21" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="47"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="62" t="s">
-        <v>18</v>
+      <c r="B22" s="57" t="s">
+        <v>17</v>
       </c>
       <c r="C22" s="7">
         <v>1</v>
       </c>
-      <c r="D22" s="46" t="s">
-        <v>58</v>
+      <c r="D22" s="42" t="s">
+        <v>48</v>
       </c>
       <c r="E22" s="21"/>
     </row>
     <row r="23" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="64"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="30">
         <v>2</v>
       </c>
-      <c r="D23" s="52" t="s">
-        <v>59</v>
+      <c r="D23" s="48" t="s">
+        <v>49</v>
       </c>
       <c r="E23" s="20"/>
     </row>
     <row r="24" spans="2:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="49">
+      <c r="B24" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="45">
         <v>1</v>
       </c>
-      <c r="D24" s="50" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="51"/>
+      <c r="D24" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="47"/>
     </row>
     <row r="25" spans="2:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="37">
+      <c r="B25" s="49" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="36">
         <v>1</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E25" s="23"/>
     </row>
@@ -2028,8 +1975,8 @@
   </sheetPr>
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2041,310 +1988,310 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="68"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="63"/>
       <c r="B3" s="2">
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="69"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="30">
         <v>7</v>
       </c>
       <c r="C4" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
         <v>4</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
-        <v>5</v>
       </c>
       <c r="B5" s="7">
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66"/>
       <c r="B6" s="2">
         <v>9</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+      <c r="C6" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
       <c r="B7" s="2">
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="72"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="30">
         <v>27</v>
       </c>
-      <c r="C8" s="43" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="62" t="s">
+      <c r="C8" s="39" t="s">
         <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="57" t="s">
+        <v>5</v>
       </c>
       <c r="B9" s="7">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
       <c r="B10" s="2">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="63"/>
+        <v>54</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="58"/>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="58"/>
       <c r="B12" s="2">
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
       <c r="B13" s="2">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
+        <v>53</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
       <c r="B14" s="2">
         <v>11</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
+        <v>55</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="58"/>
       <c r="B15" s="2">
         <v>12</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
+        <v>7</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="58"/>
       <c r="B16" s="2">
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
+        <v>56</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="58"/>
       <c r="B17" s="2">
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
+        <v>57</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="58"/>
       <c r="B18" s="2">
         <v>20</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="63"/>
+        <v>55</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="58"/>
       <c r="B19" s="2">
         <v>21</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="63"/>
+        <v>7</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="58"/>
       <c r="B20" s="2">
         <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="63"/>
+        <v>56</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="58"/>
       <c r="B21" s="2">
         <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="63"/>
+        <v>58</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="58"/>
       <c r="B22" s="2">
         <v>29</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="63"/>
+        <v>59</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="58"/>
       <c r="B23" s="2">
         <v>37</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="63"/>
+        <v>60</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="58"/>
       <c r="B24" s="2">
         <v>38</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="63"/>
+        <v>61</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="58"/>
       <c r="B25" s="2">
         <v>46</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>1</v>
+        <v>62</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="73"/>
+      <c r="A26" s="68"/>
       <c r="B26" s="11">
         <v>47</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>1</v>
+        <v>63</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2365,7 +2312,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2378,235 +2325,235 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="74" t="s">
-        <v>5</v>
+      <c r="A2" s="69" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="7">
         <v>2</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="75"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="2">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="75"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="2">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="75"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="2">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="75"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="2">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="75"/>
+      <c r="A7" s="70"/>
       <c r="B7" s="2">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="75"/>
+      <c r="A8" s="70"/>
       <c r="B8" s="2">
         <v>10</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="75"/>
+      <c r="A9" s="70"/>
       <c r="B9" s="30">
         <v>16</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>23</v>
+        <v>71</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="76" t="s">
-        <v>6</v>
+      <c r="A10" s="71" t="s">
+        <v>5</v>
       </c>
       <c r="B10" s="7">
         <v>30</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
+        <v>72</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="77"/>
+      <c r="A11" s="72"/>
       <c r="B11" s="2">
         <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="77"/>
+      <c r="A12" s="72"/>
       <c r="B12" s="2">
         <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="77"/>
+      <c r="A13" s="72"/>
       <c r="B13" s="2">
         <v>40</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="77"/>
+      <c r="A14" s="72"/>
       <c r="B14" s="2">
         <v>48</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="77"/>
+      <c r="A15" s="72"/>
       <c r="B15" s="2">
         <v>57</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="77"/>
+      <c r="A16" s="72"/>
       <c r="B16" s="2">
         <v>59</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="77"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="2">
         <v>60</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="77"/>
+      <c r="A18" s="72"/>
       <c r="B18" s="2">
         <v>63</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="77"/>
+      <c r="A19" s="72"/>
       <c r="B19" s="2">
         <v>64</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>23</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="78"/>
+      <c r="A20" s="73"/>
       <c r="B20" s="11">
         <v>22</v>
       </c>
-      <c r="C20" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>23</v>
+      <c r="C20" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2647,8 +2594,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A32"/>
+    <sheetView topLeftCell="A9" zoomScale="113" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2660,486 +2607,486 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7">
         <v>8</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="84"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79"/>
       <c r="B3" s="2">
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>25</v>
+        <v>89</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="85"/>
+      <c r="A4" s="80"/>
       <c r="B4" s="30">
         <v>13</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="70" t="s">
-        <v>5</v>
+        <v>90</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="7">
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="66"/>
       <c r="B6" s="2">
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+        <v>92</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
       <c r="B7" s="2">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
+        <v>93</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="66"/>
       <c r="B8" s="2">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="71"/>
+        <v>95</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="66"/>
       <c r="B9" s="2">
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="71"/>
+        <v>96</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="66"/>
       <c r="B10" s="2">
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="71"/>
+        <v>97</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="66"/>
       <c r="B11" s="2">
         <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="71"/>
+        <v>98</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="66"/>
       <c r="B12" s="2">
         <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>25</v>
+        <v>99</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="30">
         <v>34</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="70" t="s">
-        <v>6</v>
+        <v>94</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="65" t="s">
+        <v>5</v>
       </c>
       <c r="B14" s="7">
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="71"/>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="66"/>
       <c r="B15" s="2">
         <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="71"/>
+        <v>101</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="66"/>
       <c r="B16" s="2">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="71"/>
+        <v>102</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="66"/>
       <c r="B17" s="2">
         <v>14</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="71"/>
+        <v>100</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="66"/>
       <c r="B18" s="2">
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="71"/>
+        <v>101</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="66"/>
       <c r="B19" s="2">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="71"/>
+        <v>102</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="66"/>
       <c r="B20" s="2">
         <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="71"/>
+        <v>100</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66"/>
       <c r="B21" s="2">
         <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="71"/>
+        <v>101</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="66"/>
       <c r="B22" s="2">
         <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="71"/>
+        <v>102</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="66"/>
       <c r="B23" s="2">
         <v>32</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="71"/>
+        <v>103</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="66"/>
       <c r="B24" s="2">
         <v>41</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="71"/>
+        <v>104</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="66"/>
       <c r="B25" s="2">
         <v>49</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="71"/>
+        <v>105</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="66"/>
       <c r="B26" s="2">
         <v>50</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="71"/>
+        <v>108</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="66"/>
       <c r="B27" s="2">
         <v>51</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="71"/>
+        <v>109</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="66"/>
       <c r="B28" s="2">
         <v>61</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="71"/>
+        <v>110</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="66"/>
       <c r="B29" s="2">
         <v>65</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="71"/>
+        <v>111</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="66"/>
       <c r="B30" s="2">
         <v>72</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="71"/>
+        <v>112</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="66"/>
       <c r="B31" s="2">
         <v>73</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>25</v>
+        <v>107</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="86"/>
+      <c r="A32" s="81"/>
       <c r="B32" s="11">
         <v>80</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D32" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="79" t="s">
-        <v>17</v>
+        <v>106</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="74" t="s">
+        <v>16</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="15"/>
       <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="80"/>
+      <c r="A34" s="75"/>
       <c r="B34" s="11">
         <v>1</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="65" t="s">
-        <v>18</v>
+        <v>82</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="60" t="s">
+        <v>17</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="15"/>
       <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="81"/>
+      <c r="A36" s="76"/>
       <c r="B36" s="11">
         <v>1</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="79" t="s">
-        <v>20</v>
+        <v>83</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="74" t="s">
+        <v>19</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="15"/>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="82"/>
+    <row r="38" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="77"/>
       <c r="B38" s="2">
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>25</v>
+        <v>84</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="80"/>
+      <c r="A39" s="75"/>
       <c r="B39" s="11">
         <v>2</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="65" t="s">
-        <v>21</v>
+        <v>85</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="60" t="s">
+        <v>20</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="15"/>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="66"/>
+    <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="61"/>
       <c r="B41" s="2">
         <v>1</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D41" s="10" t="s">
-        <v>25</v>
+        <v>86</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="81"/>
+      <c r="A42" s="76"/>
       <c r="B42" s="11">
         <v>5</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>25</v>
+        <v>87</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3165,7 +3112,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3177,170 +3124,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
-        <v>5</v>
+    <row r="2" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="7">
         <v>12</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
+      <c r="A3" s="67"/>
       <c r="B3" s="30">
         <v>36</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="65" t="s">
-        <v>6</v>
+        <v>114</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="7">
         <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="66"/>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="61"/>
       <c r="B5" s="2">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
+        <v>116</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
       <c r="B6" s="2">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
+        <v>117</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61"/>
       <c r="B7" s="2">
         <v>18</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
+        <v>118</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
       <c r="B8" s="2">
         <v>26</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="66"/>
+        <v>117</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="61"/>
       <c r="B9" s="2">
         <v>27</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="66"/>
+        <v>116</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="61"/>
       <c r="B10" s="2">
         <v>52</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="66"/>
+        <v>119</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="61"/>
       <c r="B11" s="2">
         <v>66</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="66"/>
+        <v>120</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="61"/>
       <c r="B12" s="2">
         <v>67</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>24</v>
+        <v>121</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="30">
         <v>79</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>24</v>
+        <v>122</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="65" t="s">
-        <v>21</v>
+      <c r="A14" s="60" t="s">
+        <v>20</v>
       </c>
       <c r="B14" s="7">
         <v>2</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>24</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="81"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -3399,7 +3346,7 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -3412,79 +3359,79 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="15">
         <v>3</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="14">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
+      <c r="A4" s="67"/>
       <c r="B4" s="18">
         <v>16</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="65" t="s">
-        <v>5</v>
+      <c r="A5" s="60" t="s">
+        <v>4</v>
       </c>
       <c r="B5" s="15">
         <v>21</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="66"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="14">
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="66"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="18">
         <v>37</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3493,10 +3440,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3505,24 +3452,24 @@
         <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="54" t="s">
-        <v>6</v>
+      <c r="A10" s="50" t="s">
+        <v>5</v>
       </c>
       <c r="B10" s="14">
         <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3531,10 +3478,10 @@
         <v>75</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3543,26 +3490,26 @@
         <v>77</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>78</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="D13" s="34" t="s">
-        <v>10</v>
+        <v>129</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
+      <c r="A14" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3580,8 +3527,8 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3593,620 +3540,718 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="65" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="7">
         <v>5</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="71"/>
+      <c r="A3" s="66"/>
       <c r="B3" s="2">
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="71"/>
+      <c r="A4" s="66"/>
       <c r="B4" s="2">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="2">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
+      <c r="A6" s="66"/>
       <c r="B6" s="2">
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="71"/>
+      <c r="A7" s="66"/>
       <c r="B7" s="2">
         <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="71"/>
+      <c r="A8" s="66"/>
       <c r="B8" s="2">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="71"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="2">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="11">
         <v>19</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="70" t="s">
-        <v>5</v>
+        <v>138</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="65" t="s">
+        <v>4</v>
       </c>
       <c r="B11" s="7">
         <v>13</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11" s="21"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="71"/>
+        <v>139</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="66"/>
       <c r="B12" s="2">
         <v>14</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="D12" s="33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="71"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="2">
         <v>23</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13" s="17"/>
+        <v>141</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="71"/>
+      <c r="A14" s="66"/>
       <c r="B14" s="2">
         <v>24</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D14" s="17"/>
+        <v>142</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="71"/>
+      <c r="A15" s="66"/>
       <c r="B15" s="2">
         <v>25</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D15" s="17"/>
+        <v>143</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="71"/>
+      <c r="A16" s="66"/>
       <c r="B16" s="2">
         <v>29</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="D16" s="17"/>
+        <v>144</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="71"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="2">
         <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D17" s="17"/>
+        <v>145</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="71"/>
+      <c r="A18" s="66"/>
       <c r="B18" s="2">
         <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D18" s="17"/>
+        <v>146</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="71"/>
+      <c r="A19" s="66"/>
       <c r="B19" s="2">
         <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D19" s="17"/>
+        <v>147</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="71"/>
+      <c r="A20" s="66"/>
       <c r="B20" s="2">
         <v>35</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D20" s="17"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="71"/>
+        <v>148</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66"/>
       <c r="B21" s="2">
         <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="D21" s="17"/>
+        <v>149</v>
+      </c>
+      <c r="D21" s="33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="71"/>
+      <c r="A22" s="66"/>
       <c r="B22" s="2">
         <v>39</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D22" s="17"/>
+        <v>150</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="86"/>
+      <c r="A23" s="81"/>
       <c r="B23" s="11">
         <v>40</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="D23" s="34"/>
+        <v>151</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="90" t="s">
-        <v>6</v>
+      <c r="A24" s="85" t="s">
+        <v>5</v>
       </c>
       <c r="B24" s="28">
         <v>34</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>162</v>
-      </c>
-      <c r="D24" s="41"/>
+        <v>152</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="90"/>
+      <c r="A25" s="85"/>
       <c r="B25" s="2">
         <v>35</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D25" s="39"/>
+        <v>153</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="90"/>
+      <c r="A26" s="85"/>
       <c r="B26" s="2">
         <v>43</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="D26" s="39"/>
+        <v>154</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="90"/>
+      <c r="A27" s="85"/>
       <c r="B27" s="2">
         <v>44</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D27" s="39"/>
+        <v>155</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="90"/>
+      <c r="A28" s="85"/>
       <c r="B28" s="2">
         <v>53</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D28" s="39"/>
+        <v>156</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="90"/>
+      <c r="A29" s="85"/>
       <c r="B29" s="2">
         <v>54</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="D29" s="39"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="90"/>
+        <v>157</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="85"/>
       <c r="B30" s="2">
         <v>58</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="D30" s="39"/>
+        <v>158</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="90"/>
+      <c r="A31" s="85"/>
       <c r="B31" s="2">
         <v>62</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D31" s="39"/>
+        <v>159</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="90"/>
+      <c r="A32" s="85"/>
       <c r="B32" s="2">
         <v>69</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="D32" s="39"/>
+        <v>160</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
+      <c r="A33" s="85"/>
       <c r="B33" s="2">
         <v>74</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D33" s="39"/>
+        <v>161</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="90"/>
+      <c r="A34" s="85"/>
       <c r="B34" s="30">
         <v>76</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="40"/>
+        <v>162</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="91" t="s">
-        <v>17</v>
+      <c r="A35" s="86" t="s">
+        <v>16</v>
       </c>
       <c r="B35" s="7">
         <v>2</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D35" s="21"/>
+        <v>163</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="92"/>
+      <c r="A36" s="87"/>
       <c r="B36" s="2">
         <v>3</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D36" s="17"/>
+        <v>164</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="93"/>
+      <c r="A37" s="88"/>
       <c r="B37" s="11">
         <v>4</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D37" s="34"/>
+        <v>165</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="87" t="s">
-        <v>18</v>
+      <c r="A38" s="82" t="s">
+        <v>17</v>
       </c>
       <c r="B38" s="7">
         <v>2</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D38" s="21"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="88"/>
+        <v>166</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="83"/>
       <c r="B39" s="2">
         <v>3</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D39" s="17"/>
+        <v>167</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="88"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="2">
         <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D40" s="17"/>
+        <v>168</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="89"/>
+      <c r="A41" s="84"/>
       <c r="B41" s="30">
         <v>6</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="D41" s="20"/>
+        <v>169</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="91" t="s">
-        <v>19</v>
+      <c r="A42" s="86" t="s">
+        <v>18</v>
       </c>
       <c r="B42" s="7">
         <v>1</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="D42" s="21"/>
+        <v>170</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="92"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="2">
         <v>2</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="D43" s="17"/>
+        <v>171</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="92"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="2">
         <v>3</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D44" s="17"/>
+        <v>172</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="92"/>
+      <c r="A45" s="87"/>
       <c r="B45" s="2">
         <v>4</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D45" s="17"/>
+        <v>173</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="92"/>
+      <c r="A46" s="87"/>
       <c r="B46" s="2">
         <v>5</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D46" s="17"/>
+        <v>174</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="92"/>
+      <c r="A47" s="87"/>
       <c r="B47" s="2">
         <v>6</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="D47" s="17"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="92"/>
+        <v>175</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="87"/>
       <c r="B48" s="2">
         <v>7</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="D48" s="17"/>
+        <v>176</v>
+      </c>
+      <c r="D48" s="33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="92"/>
+      <c r="A49" s="87"/>
       <c r="B49" s="2">
         <v>8</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="D49" s="17"/>
+        <v>177</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="50" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="93"/>
+      <c r="A50" s="88"/>
       <c r="B50" s="30">
         <v>9</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="D50" s="20"/>
+        <v>178</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="87" t="s">
-        <v>20</v>
+      <c r="A51" s="82" t="s">
+        <v>19</v>
       </c>
       <c r="B51" s="7">
         <v>3</v>
       </c>
       <c r="C51" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D51" s="21"/>
+        <v>179</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="88"/>
+      <c r="A52" s="83"/>
       <c r="B52" s="2">
         <v>4</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D52" s="17"/>
+        <v>180</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="88"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="2">
         <v>5</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D53" s="17"/>
+        <v>181</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="89"/>
+      <c r="A54" s="84"/>
       <c r="B54" s="30">
         <v>6</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>192</v>
-      </c>
-      <c r="D54" s="20"/>
+        <v>182</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="87" t="s">
-        <v>21</v>
+      <c r="A55" s="82" t="s">
+        <v>20</v>
       </c>
       <c r="B55" s="7">
         <v>3</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>193</v>
-      </c>
-      <c r="D55" s="21"/>
+        <v>183</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="88"/>
+      <c r="A56" s="83"/>
       <c r="B56" s="2">
         <v>4</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="D56" s="17"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="88"/>
+        <v>184</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="83"/>
       <c r="B57" s="2">
         <v>6</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D57" s="17"/>
+        <v>185</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="58" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="88"/>
+      <c r="A58" s="83"/>
       <c r="B58" s="30">
         <v>7</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>196</v>
-      </c>
-      <c r="D58" s="20"/>
+        <v>186</v>
+      </c>
+      <c r="D58" s="20" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="59" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="37">
+        <v>21</v>
+      </c>
+      <c r="B59" s="36">
         <v>2</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D59" s="23"/>
+        <v>187</v>
+      </c>
+      <c r="D59" s="23" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4226,203 +4271,200 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14301F0A-C59F-4D53-B805-8A2C0910161F}">
-  <dimension ref="B1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D601B1C-2631-CB42-BD6D-45A4239C91A4}">
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1"/>
-    <col min="4" max="4" width="66.1640625" style="55" customWidth="1"/>
+    <col min="1" max="1" width="49.1640625" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B2" s="70" t="s">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7">
+        <v>26</v>
+      </c>
+      <c r="C2" s="51" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="67"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7">
-        <v>26</v>
-      </c>
-      <c r="D2" s="56" t="s">
+      <c r="B4" s="7">
+        <v>36</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="66"/>
+      <c r="B5" s="2">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="66"/>
+      <c r="B6" s="2">
+        <v>55</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="33" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="66"/>
+      <c r="B7" s="2">
+        <v>56</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A8" s="66"/>
+      <c r="B8" s="2">
+        <v>70</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="81"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="89" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="28">
+        <v>5</v>
+      </c>
+      <c r="C10" s="55" t="s">
+        <v>194</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="81"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5</v>
+      </c>
+      <c r="C12" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="81"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="33"/>
+    </row>
+    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="7">
+        <v>10</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="58"/>
+      <c r="B15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="33"/>
+    </row>
+    <row r="17" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="36">
+        <v>7</v>
+      </c>
+      <c r="C17" s="56" t="s">
         <v>198</v>
       </c>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="72"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B4" s="70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="7">
-        <v>36</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>199</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B5" s="71"/>
-      <c r="C5" s="2">
-        <v>45</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B6" s="71"/>
-      <c r="C6" s="2">
-        <v>55</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B7" s="71"/>
-      <c r="C7" s="2">
-        <v>56</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B8" s="71"/>
-      <c r="C8" s="2">
-        <v>70</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="86"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="34"/>
-    </row>
-    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B10" s="94" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="28">
-        <v>5</v>
-      </c>
-      <c r="D10" s="60" t="s">
-        <v>204</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="86"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="34"/>
-    </row>
-    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B12" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="7">
-        <v>5</v>
-      </c>
-      <c r="D12" s="58" t="s">
-        <v>205</v>
-      </c>
-      <c r="E12" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="86"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="34"/>
-    </row>
-    <row r="14" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B14" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="7">
-        <v>10</v>
-      </c>
-      <c r="D14" s="58" t="s">
+      <c r="D17" s="21" t="s">
         <v>206</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="63"/>
-      <c r="C15" s="2">
-        <v>11</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="73"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="34"/>
-    </row>
-    <row r="17" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="37">
-        <v>7</v>
-      </c>
-      <c r="D17" s="61" t="s">
-        <v>208</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>